<commit_message>
update example clinical info
</commit_message>
<xml_diff>
--- a/data/test_data/test_clinical_data.xlsx
+++ b/data/test_data/test_clinical_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarzec/Documents/GitHub/UMCCR/RNAseq-Analysis-Report/data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FD7B4B-AA74-C54E-A796-FBBF9707653D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1D353A-61EF-9347-91B8-818222D09F6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2220" windowWidth="28800" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31720" yWindow="6180" windowWidth="28800" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,10 +422,10 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -505,19 +505,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1">
-        <v>42871</v>
+        <v>42537</v>
       </c>
       <c r="D2" s="1">
-        <v>43034</v>
+        <v>42761</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="1">
-        <v>42895</v>
+        <v>42956</v>
       </c>
       <c r="G2" s="1">
-        <v>43000</v>
+        <v>43116</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Use <Subject_ID>__<SampleName> convention for expected umccrise output data
</commit_message>
<xml_diff>
--- a/data/test_data/test_clinical_data.xlsx
+++ b/data/test_data/test_clinical_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarzec/Documents/GitHub/UMCCR/RNAseq-Analysis-Report/data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6A667E-D5C7-5440-B229-54E035A8453F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0246E0-2B30-E24D-AC5C-CEBAAA772143}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="10100" windowWidth="28800" windowHeight="7040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34840" yWindow="5420" windowWidth="28800" windowHeight="7040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Subject ID</t>
   </si>
   <si>
-    <t>test.subject</t>
-  </si>
-  <si>
     <t>Irinotecan</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Oxaliplatin, Other</t>
+  </si>
+  <si>
+    <t>test_subject</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,10 +499,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>42537</v>
@@ -511,7 +511,7 @@
         <v>42761</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1">
         <v>42956</v>
@@ -529,7 +529,7 @@
         <v>42879</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1">
         <v>43206</v>
@@ -538,7 +538,7 @@
         <v>43271</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="1">
         <v>43298</v>

</xml_diff>

<commit_message>
Update test clinical data
</commit_message>
<xml_diff>
--- a/data/test_data/test_clinical_data.xlsx
+++ b/data/test_data/test_clinical_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarzec/Documents/GitHub/UMCCR/RNAseq-Analysis-Report/data/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarzec/Documents/GitHub/UMCCR/RNAsum/data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0246E0-2B30-E24D-AC5C-CEBAAA772143}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40513783-1E6B-3C49-A95D-F7CEFB38A9A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34840" yWindow="5420" windowWidth="28800" windowHeight="7040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t/>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>test_subject</t>
+  </si>
+  <si>
+    <t>test_subject__test_sample</t>
   </si>
 </sst>
 </file>
@@ -419,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,6 +550,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42537</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42761</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1">
+        <v>42956</v>
+      </c>
+      <c r="G3" s="1">
+        <v>43116</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42797</v>
+      </c>
+      <c r="J3" s="1">
+        <v>42879</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <v>43206</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43271</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="1">
+        <v>43298</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:P2" xr:uid="{91CF9853-88B9-4658-B4FC-B6D9058A01EB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>